<commit_message>
study: bugfix field not added in form
Change headers in excel file

Update date format in date picker
</commit_message>
<xml_diff>
--- a/src/assets/upload_examples/observations_in_columns.xlsx
+++ b/src/assets/upload_examples/observations_in_columns.xlsx
@@ -22,10 +22,10 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="9">
   <si>
-    <t xml:space="preserve">Accession</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Study</t>
+    <t xml:space="preserve">ACCESSION</t>
+  </si>
+  <si>
+    <t xml:space="preserve">STUDY</t>
   </si>
   <si>
     <t xml:space="preserve">Plant size:cm</t>
@@ -159,19 +159,17 @@
   <dimension ref="A1:J31"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2:D4"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="24.35"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="11.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="7.41"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="7" min="6" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="38.76"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="9" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>